<commit_message>
updated map and project info
</commit_message>
<xml_diff>
--- a/docs/Project_Info/Project_Info.xlsx
+++ b/docs/Project_Info/Project_Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\imas-flathead-io\docs\Project_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35DD505-1850-4FD1-B1D7-FE8E52A30179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F87C2B-3829-4735-9DAE-43CEE8FF5D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{0A3BEAC7-50BE-44D8-8B3D-5734D11E2F12}"/>
+    <workbookView xWindow="3234" yWindow="936" windowWidth="13422" windowHeight="12246" xr2:uid="{0A3BEAC7-50BE-44D8-8B3D-5734D11E2F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Issue</t>
   </si>
@@ -79,6 +79,30 @@
   </si>
   <si>
     <t xml:space="preserve">For now, for demonstration purposes, any management advice is assumed to be followed exactly </t>
+  </si>
+  <si>
+    <t>Nominal Effort could be improved as an index of exploitation rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can we derive effort / habitat area. There is the potential to borrow information on catchability among areas/models - priors, metaanalysis, EM. </t>
+  </si>
+  <si>
+    <t>Catches are expanded to totals using expansion factor - no uncertainty</t>
+  </si>
+  <si>
+    <t>How can we get observation error in total catches? How are expansion factors calculated - can we do bootstrapping etc?</t>
+  </si>
+  <si>
+    <t>Discard mortality rate assumed to be 9% but from a study elsehwere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lyle et al. 2006.  This is used to include discard mortality in total catch data (in model conditioning [Catch = ExpFac x (Kept + Rel * DiscMort)] and used in projections that would affect any kind of regulation affecting discarding such as size limits, bag limits etc. </t>
+  </si>
+  <si>
+    <t>Total recreational effort</t>
+  </si>
+  <si>
+    <t>currently calculated by Duration_hrs x Npersons x ExpWt (what is the 'expansion factor'??)</t>
   </si>
 </sst>
 </file>
@@ -447,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54945D8-9D04-4CC7-AA85-EDE6405E2E30}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B18" sqref="B17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -532,6 +556,38 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Maturity figures, regs doc
</commit_message>
<xml_diff>
--- a/docs/Project_Info/Project_Info.xlsx
+++ b/docs/Project_Info/Project_Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\imas-flathead-io\docs\Project_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2C0DA5-4AB1-4756-B33F-5AF232585508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BC16B9-EF5A-46CD-AC8E-D00B545EB3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="4026" windowWidth="19530" windowHeight="7218" xr2:uid="{0A3BEAC7-50BE-44D8-8B3D-5734D11E2F12}"/>
+    <workbookView xWindow="1368" yWindow="3060" windowWidth="19530" windowHeight="12246" xr2:uid="{0A3BEAC7-50BE-44D8-8B3D-5734D11E2F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Issue</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Is this correct, for all areas?</t>
   </si>
   <si>
-    <t>From an online report by NRE ('around 27 cm')</t>
-  </si>
-  <si>
     <t>Background rate of discarding</t>
   </si>
   <si>
@@ -108,30 +105,18 @@
     <t>SEC</t>
   </si>
   <si>
-    <t>Derwent Estuary, Tasman, Frederick Henry/Norfolk Bay, South-eastern coast, D'entrecasteaux Channel, South</t>
-  </si>
-  <si>
     <t>EC</t>
   </si>
   <si>
-    <t>Great Oyster Bay, Central-eastern coast, Eastern coast</t>
-  </si>
-  <si>
     <t>NWC</t>
   </si>
   <si>
-    <t>North-western coast, King Island</t>
-  </si>
-  <si>
     <t>NEC</t>
   </si>
   <si>
     <t>WC</t>
   </si>
   <si>
-    <t>Tamar River, North-eastern coast, Flinders Island</t>
-  </si>
-  <si>
     <t>Central-western coast, Western coast, South-western coast</t>
   </si>
   <si>
@@ -154,6 +139,33 @@
   </si>
   <si>
     <t>Recreational survey index by large region is standardized as a linear model</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Derwent Estuary, Tasman, Frederick Henry/Norfolk Bay, South-eastern coast, D'entrecasteaux Channel, South, Northwest Bay, SECest, SEC</t>
+  </si>
+  <si>
+    <t>Great Oyster Bay, Central-eastern coast, Eastern coast, Coles Bay, Georges Bay, EC</t>
+  </si>
+  <si>
+    <t>North-western coast, King Island, rocky cape, NWC</t>
+  </si>
+  <si>
+    <t>EAT, ECS, ET, SET, CBS, no sample</t>
+  </si>
+  <si>
+    <t>From an online report by NRE ('around 27 cm') - but actually there is GonadState, Gonadweightand Statge Mature 3-7, in the historical data (how to interpret these?). StageMature 3-7 is 50% at length 31cm in the data (aggregated)</t>
+  </si>
+  <si>
+    <t>Tamar River, North-eastern coast, Flinders Island, Spring Bay, Flinders/Eastcoast, NC, EC, Deal island, Hogan group, NEC, FI</t>
+  </si>
+  <si>
+    <t>Not clear how to assign calendar year to commercial year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currently this is assumed to occur mostly in the second half, ie Nov 1 - Sep 1, so 2022/23 would be assigned the year 2023. </t>
   </si>
 </sst>
 </file>
@@ -525,16 +537,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54945D8-9D04-4CC7-AA85-EDE6405E2E30}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="34.62890625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="66.9453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="82.83984375" style="3" customWidth="1"/>
     <col min="3" max="16384" width="8.83984375" style="2"/>
   </cols>
   <sheetData>
@@ -546,12 +558,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -580,135 +592,151 @@
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First splash page shared
</commit_message>
<xml_diff>
--- a/docs/Project_Info/Project_Info.xlsx
+++ b/docs/Project_Info/Project_Info.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1371" yWindow="3060" windowWidth="19534" windowHeight="12249"/>
+    <workbookView xWindow="1371" yWindow="3060" windowWidth="19534" windowHeight="12249" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
+    <sheet name="Todo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Issue</t>
   </si>
@@ -182,10 +183,49 @@
     <t>The RCM model requires either complete effort or complete catches. For now I just linearly interpolated / constantly extrapolated catches. Maybe move to an effort model next?</t>
   </si>
   <si>
-    <t>Commercial fishery exploitation is unknown</t>
-  </si>
-  <si>
     <t>For now I'm assuming it follows the survey comp data</t>
+  </si>
+  <si>
+    <t>Commercial fishery selectivity / retention is unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM fleet and survey structure: </t>
+  </si>
+  <si>
+    <t>2 fleets (rec / commercial), 4 surveys (rec CPUE, commercial CPUE, historial length/age comp, rec survey length/age comp)</t>
+  </si>
+  <si>
+    <t>Fleet seleectivities are not informed by length / age data</t>
+  </si>
+  <si>
+    <t>Currently specified - but can we assume that the rec survey reflects the recreational fishery? If so then we can move around the data to make the rec selectivity / CPUE informated by the same length/age observations</t>
+  </si>
+  <si>
+    <t>Model arbitarily started in 1974 (50 historical years)</t>
+  </si>
+  <si>
+    <t>What is a suitable time to start fishing?</t>
+  </si>
+  <si>
+    <t>Equilibrium catches assumed to be negligible before 1974 (again arbitrarily) of those observed</t>
+  </si>
+  <si>
+    <t>C_eq = 0.00001 * mean historical catch but can bring forward the initial model year and specify a differing C_eq</t>
+  </si>
+  <si>
+    <t>Data weighting profiling</t>
+  </si>
+  <si>
+    <t>Parameter profiling</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Meet to discuss straw-dog fits</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -557,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -644,146 +684,221 @@
     </row>
     <row r="10" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="4" t="s">
-        <v>50</v>
+      <c r="A19" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
-        <v>52</v>
+      <c r="A20" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.53515625" customWidth="1"/>
+    <col min="2" max="2" width="27.4609375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest splash page post revision
</commit_message>
<xml_diff>
--- a/docs/Project_Info/Project_Info.xlsx
+++ b/docs/Project_Info/Project_Info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcarruth\Documents\GitHub\imas-flathead-io\docs\Project_Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\imas-flathead-io\docs\Project_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872EEDAD-6A07-475B-A6C7-E056859B75E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1371" yWindow="3060" windowWidth="19534" windowHeight="12249" activeTab="1"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="16362" windowHeight="9654" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues" sheetId="1" r:id="rId1"/>
@@ -90,9 +91,6 @@
     <t>How can we get observation error in total catches? How are expansion factors calculated - can we do bootstrapping etc?</t>
   </si>
   <si>
-    <t>Discard mortality rate assumed to be 9% but from a study elsehwere</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lyle et al. 2006.  This is used to include discard mortality in total catch data (in model conditioning [Catch = ExpFac x (Kept + Rel * DiscMort)] and used in projections that would affect any kind of regulation affecting discarding such as size limits, bag limits etc. </t>
   </si>
   <si>
@@ -198,9 +196,6 @@
     <t>Fleet seleectivities are not informed by length / age data</t>
   </si>
   <si>
-    <t>Currently specified - but can we assume that the rec survey reflects the recreational fishery? If so then we can move around the data to make the rec selectivity / CPUE informated by the same length/age observations</t>
-  </si>
-  <si>
     <t>Model arbitarily started in 1974 (50 historical years)</t>
   </si>
   <si>
@@ -226,12 +221,18 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>we assume that the rec survey reflects the recreational fishery</t>
+  </si>
+  <si>
+    <t>Discard mortality rate assumed to be 6% as the max from deep water estimates of Lyle et al 2006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -596,21 +597,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="34.61328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="82.84375" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="8.84375" style="2"/>
+    <col min="1" max="1" width="34.62890625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="82.83984375" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="8.83984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,15 +619,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -634,7 +635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -642,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -650,7 +651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -658,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -666,7 +667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -674,7 +675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -682,39 +683,39 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -722,7 +723,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -730,132 +731,132 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
+      <c r="B26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -864,41 +865,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.53515625" customWidth="1"/>
-    <col min="2" max="2" width="27.4609375" customWidth="1"/>
+    <col min="1" max="1" width="22.5234375" customWidth="1"/>
+    <col min="2" max="2" width="27.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
       <c r="B2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>